<commit_message>
Fixed close and reactivate incident use-cases.
</commit_message>
<xml_diff>
--- a/DOCS/Use Cases/Estimations of use cases and complition status.xlsx
+++ b/DOCS/Use Cases/Estimations of use cases and complition status.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>UC</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>UUCW</t>
+  </si>
+  <si>
+    <t>Reactivate incident</t>
   </si>
 </sst>
 </file>
@@ -499,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -547,8 +550,8 @@
         <v>10</v>
       </c>
       <c r="F2" s="2">
-        <f>E2/E37</f>
-        <v>0.04</v>
+        <f>E2/E38</f>
+        <v>3.9215686274509803E-2</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -566,18 +569,18 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E34" si="0">B3*5+C3*10+D3*15</f>
+        <f t="shared" ref="E3:E35" si="0">B3*5+C3*10+D3*15</f>
         <v>10</v>
       </c>
       <c r="F3" s="2">
-        <f>E3/E37</f>
-        <v>0.04</v>
+        <f>E3/E38</f>
+        <v>3.9215686274509803E-2</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I34" si="1">E3*H3</f>
+        <f t="shared" ref="I3:I35" si="1">E3*H3</f>
         <v>10</v>
       </c>
     </row>
@@ -593,8 +596,8 @@
         <v>5</v>
       </c>
       <c r="F4" s="2">
-        <f>E4/E37</f>
-        <v>0.02</v>
+        <f>E4/E38</f>
+        <v>1.9607843137254902E-2</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -616,8 +619,8 @@
         <v>10</v>
       </c>
       <c r="F5" s="2">
-        <f>E5/E37</f>
-        <v>0.04</v>
+        <f>E5/E38</f>
+        <v>3.9215686274509803E-2</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -639,8 +642,8 @@
         <v>10</v>
       </c>
       <c r="F6" s="2">
-        <f>E6/E37</f>
-        <v>0.04</v>
+        <f>E6/E38</f>
+        <v>3.9215686274509803E-2</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -662,8 +665,8 @@
         <v>10</v>
       </c>
       <c r="F7" s="2">
-        <f>E7/E37</f>
-        <v>0.04</v>
+        <f>E7/E38</f>
+        <v>3.9215686274509803E-2</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -685,8 +688,8 @@
         <v>10</v>
       </c>
       <c r="F8" s="2">
-        <f>E8/E37</f>
-        <v>0.04</v>
+        <f>E8/E38</f>
+        <v>3.9215686274509803E-2</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -708,8 +711,8 @@
         <v>10</v>
       </c>
       <c r="F9" s="2">
-        <f>E9/E37</f>
-        <v>0.04</v>
+        <f>E9/E38</f>
+        <v>3.9215686274509803E-2</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -731,8 +734,8 @@
         <v>5</v>
       </c>
       <c r="F10" s="2">
-        <f>E10/E37</f>
-        <v>0.02</v>
+        <f>E10/E38</f>
+        <v>1.9607843137254902E-2</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -754,8 +757,8 @@
         <v>5</v>
       </c>
       <c r="F11" s="2">
-        <f>E11/E37</f>
-        <v>0.02</v>
+        <f>E11/E38</f>
+        <v>1.9607843137254902E-2</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -777,8 +780,8 @@
         <v>5</v>
       </c>
       <c r="F12" s="2">
-        <f>E12/E37</f>
-        <v>0.02</v>
+        <f>E12/E38</f>
+        <v>1.9607843137254902E-2</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -800,8 +803,8 @@
         <v>5</v>
       </c>
       <c r="F13" s="2">
-        <f>E13/E37</f>
-        <v>0.02</v>
+        <f>E13/E38</f>
+        <v>1.9607843137254902E-2</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -823,8 +826,8 @@
         <v>5</v>
       </c>
       <c r="F14" s="2">
-        <f>E14/E37</f>
-        <v>0.02</v>
+        <f>E14/E38</f>
+        <v>1.9607843137254902E-2</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -846,8 +849,8 @@
         <v>5</v>
       </c>
       <c r="F15" s="2">
-        <f>E15/E37</f>
-        <v>0.02</v>
+        <f>E15/E38</f>
+        <v>1.9607843137254902E-2</v>
       </c>
       <c r="I15">
         <f t="shared" si="1"/>
@@ -866,8 +869,8 @@
         <v>15</v>
       </c>
       <c r="F16" s="2">
-        <f>E16/E37</f>
-        <v>0.06</v>
+        <f>E16/E38</f>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -889,8 +892,8 @@
         <v>10</v>
       </c>
       <c r="F17" s="2">
-        <f>E17/E37</f>
-        <v>0.04</v>
+        <f>E17/E38</f>
+        <v>3.9215686274509803E-2</v>
       </c>
       <c r="H17">
         <v>1</v>
@@ -912,8 +915,8 @@
         <v>15</v>
       </c>
       <c r="F18" s="2">
-        <f>E18/E37</f>
-        <v>0.06</v>
+        <f>E18/E38</f>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="H18">
         <v>1</v>
@@ -935,8 +938,8 @@
         <v>5</v>
       </c>
       <c r="F19" s="2">
-        <f>E19/E37</f>
-        <v>0.02</v>
+        <f>E19/E38</f>
+        <v>1.9607843137254902E-2</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -958,8 +961,8 @@
         <v>10</v>
       </c>
       <c r="F20" s="2">
-        <f>E20/E37</f>
-        <v>0.04</v>
+        <f>E20/E38</f>
+        <v>3.9215686274509803E-2</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -981,8 +984,8 @@
         <v>5</v>
       </c>
       <c r="F21" s="2">
-        <f>E21/E37</f>
-        <v>0.02</v>
+        <f>E21/E38</f>
+        <v>1.9607843137254902E-2</v>
       </c>
       <c r="H21">
         <v>1</v>
@@ -1004,8 +1007,8 @@
         <v>5</v>
       </c>
       <c r="F22" s="2">
-        <f>E22/E37</f>
-        <v>0.02</v>
+        <f>E22/E38</f>
+        <v>1.9607843137254902E-2</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -1027,8 +1030,8 @@
         <v>5</v>
       </c>
       <c r="F23" s="2">
-        <f>E23/E37</f>
-        <v>0.02</v>
+        <f>E23/E38</f>
+        <v>1.9607843137254902E-2</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -1050,8 +1053,8 @@
         <v>10</v>
       </c>
       <c r="F24" s="2">
-        <f>E24/E37</f>
-        <v>0.04</v>
+        <f>E24/E38</f>
+        <v>3.9215686274509803E-2</v>
       </c>
       <c r="H24">
         <v>1</v>
@@ -1069,47 +1072,47 @@
         <v>1</v>
       </c>
       <c r="E25">
-        <f t="shared" si="0"/>
+        <f>B25*5+C25*10+D25*15</f>
         <v>10</v>
       </c>
       <c r="F25" s="2">
-        <f>E25/E37</f>
-        <v>0.04</v>
+        <f>E25/E38</f>
+        <v>3.9215686274509803E-2</v>
       </c>
       <c r="H25">
         <v>1</v>
       </c>
       <c r="I25">
-        <f t="shared" si="1"/>
+        <f>E25*H25</f>
         <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="E26">
-        <f t="shared" si="0"/>
+        <f>B26*5+C26*10+D26*15</f>
         <v>5</v>
       </c>
       <c r="F26" s="2">
-        <f>E26/E37</f>
-        <v>0.02</v>
+        <f>E26/E38</f>
+        <v>1.9607843137254902E-2</v>
       </c>
       <c r="H26">
         <v>1</v>
       </c>
       <c r="I26">
-        <f t="shared" si="1"/>
+        <f>E26*H26</f>
         <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -1119,8 +1122,8 @@
         <v>5</v>
       </c>
       <c r="F27" s="2">
-        <f>E27/E37</f>
-        <v>0.02</v>
+        <f>E27/E38</f>
+        <v>1.9607843137254902E-2</v>
       </c>
       <c r="H27">
         <v>1</v>
@@ -1132,7 +1135,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -1142,17 +1145,20 @@
         <v>5</v>
       </c>
       <c r="F28" s="2">
-        <f>E28/E37</f>
-        <v>0.02</v>
+        <f>E28/E38</f>
+        <v>1.9607843137254902E-2</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
       </c>
       <c r="I28">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -1162,8 +1168,8 @@
         <v>5</v>
       </c>
       <c r="F29" s="2">
-        <f>E29/E37</f>
-        <v>0.02</v>
+        <f>E29/E38</f>
+        <v>1.9607843137254902E-2</v>
       </c>
       <c r="I29">
         <f t="shared" si="1"/>
@@ -1172,7 +1178,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -1182,8 +1188,8 @@
         <v>5</v>
       </c>
       <c r="F30" s="2">
-        <f>E30/E37</f>
-        <v>0.02</v>
+        <f>E30/E38</f>
+        <v>1.9607843137254902E-2</v>
       </c>
       <c r="I30">
         <f t="shared" si="1"/>
@@ -1192,7 +1198,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -1202,8 +1208,8 @@
         <v>5</v>
       </c>
       <c r="F31" s="2">
-        <f>E31/E37</f>
-        <v>0.02</v>
+        <f>E31/E38</f>
+        <v>1.9607843137254902E-2</v>
       </c>
       <c r="I31">
         <f t="shared" si="1"/>
@@ -1212,7 +1218,7 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -1222,8 +1228,8 @@
         <v>5</v>
       </c>
       <c r="F32" s="2">
-        <f>E32/E37</f>
-        <v>0.02</v>
+        <f>E32/E38</f>
+        <v>1.9607843137254902E-2</v>
       </c>
       <c r="I32">
         <f t="shared" si="1"/>
@@ -1232,82 +1238,102 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>37</v>
-      </c>
-      <c r="C33">
+        <v>36</v>
+      </c>
+      <c r="B33">
         <v>1</v>
       </c>
       <c r="E33">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F33" s="2">
-        <f>E33/E37</f>
-        <v>0.04</v>
-      </c>
-      <c r="H33">
-        <v>1</v>
+        <f>E33/E38</f>
+        <v>1.9607843137254902E-2</v>
       </c>
       <c r="I33">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F34" s="2">
+        <f>E34/E38</f>
+        <v>3.9215686274509803E-2</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" t="s">
         <v>38</v>
       </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-      <c r="E34">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="F34" s="2">
-        <f>E34/E37</f>
-        <v>0.04</v>
-      </c>
-      <c r="I34">
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F35" s="2">
+        <f>E35/E38</f>
+        <v>3.9215686274509803E-2</v>
+      </c>
+      <c r="I35">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
-      <c r="A37" t="s">
+    <row r="38" spans="1:10">
+      <c r="A38" t="s">
         <v>39</v>
       </c>
-      <c r="B37">
-        <f>SUM(B2:B36)*5</f>
-        <v>90</v>
-      </c>
-      <c r="C37">
-        <f>SUM(C2:C36)*10</f>
+      <c r="B38">
+        <f>SUM(B2:B37)*5</f>
+        <v>95</v>
+      </c>
+      <c r="C38">
+        <f>SUM(C2:C37)*10</f>
         <v>130</v>
       </c>
-      <c r="D37">
-        <f>SUM(D2:D36)*15</f>
+      <c r="D38">
+        <f>SUM(D2:D37)*15</f>
         <v>30</v>
       </c>
-      <c r="E37">
-        <f>SUM(B37:D37)</f>
-        <v>250</v>
-      </c>
-      <c r="F37" s="2">
-        <f>SUM(F2:F36)</f>
-        <v>1.0000000000000004</v>
-      </c>
-      <c r="H37">
-        <f>SUM(H2:H36)</f>
-        <v>26</v>
-      </c>
-      <c r="I37">
-        <f>SUM(I2:I36)</f>
-        <v>210</v>
-      </c>
-      <c r="J37">
-        <f>I37*F37/E37</f>
-        <v>0.8400000000000003</v>
+      <c r="E38">
+        <f>SUM(B38:D38)</f>
+        <v>255</v>
+      </c>
+      <c r="F38" s="2">
+        <f>SUM(F2:F37)</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="H38">
+        <f>SUM(H2:H37)</f>
+        <v>27</v>
+      </c>
+      <c r="I38">
+        <f>SUM(I2:I37)</f>
+        <v>215</v>
+      </c>
+      <c r="J38">
+        <f>I38*F38/E38</f>
+        <v>0.84313725490196101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>